<commit_message>
exploration of buffered audio
</commit_message>
<xml_diff>
--- a/hoursLog.xlsx
+++ b/hoursLog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>date</t>
   </si>
@@ -33,7 +33,13 @@
     <t>2020.02.08</t>
   </si>
   <si>
-    <t>working on getting min-devkit environment setup</t>
+    <t xml:space="preserve">working on getting min-devkit environment setup. Big compiler issues with cmake. Had to do this: had to do this: https://stackoverflow.com/questions/17980759/xcode-select-active-developer-directory-error/17980786#17980786. </t>
+  </si>
+  <si>
+    <t>2020.02.22</t>
+  </si>
+  <si>
+    <t>Went through two buffer Max examples. Have yet to go through corresponding code throroughly. Read through GuideToAudio.md. Read through c74_min_operator_vector.h, which contains critical information about the audio_bundle object.</t>
   </si>
 </sst>
 </file>
@@ -69,8 +75,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,15 +411,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -420,19 +429,30 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" ht="54" customHeight="1">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
         <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="45">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>1.5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reacquainting with organization; learning to make new project
you can make a new project using Max
</commit_message>
<xml_diff>
--- a/hoursLog.xlsx
+++ b/hoursLog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>date</t>
   </si>
@@ -40,6 +40,18 @@
   </si>
   <si>
     <t>Went through two buffer Max examples. Have yet to go through corresponding code throroughly. Read through GuideToAudio.md. Read through c74_min_operator_vector.h, which contains critical information about the audio_bundle object.</t>
+  </si>
+  <si>
+    <t>meeting with Konrad</t>
+  </si>
+  <si>
+    <t>2020.04.23</t>
+  </si>
+  <si>
+    <t>2020.05.04</t>
+  </si>
+  <si>
+    <t>total</t>
   </si>
 </sst>
 </file>
@@ -75,11 +87,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,48 +424,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="78.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="78.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="54" customHeight="1">
+    <row r="2" spans="1:5" ht="54" customHeight="1">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="D2" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="45">
+    </row>
+    <row r="3" spans="1:5" ht="45">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>1.5</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="D4" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D6" s="2">
+        <f>C6-B6</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="2">
+        <f xml:space="preserve"> SUM(D2:D31)</f>
+        <v>0.35416666666666663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
now able to build a new project, and build new objects within that project, using the Xcode IDE
note that you can also build a new project from Max, but it was unclear to where in that process you are supposed to build, cause it doesn't do that automatically
</commit_message>
<xml_diff>
--- a/hoursLog.xlsx
+++ b/hoursLog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>date</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>reacquainting myself with min organization, setting up any connect for max</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -495,11 +498,19 @@
         <v>0.5</v>
       </c>
       <c r="C6" s="2">
-        <v>0.54166666666666663</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="D6" s="2">
         <f>C6-B6</f>
-        <v>4.166666666666663E-2</v>
+        <v>0.10416666666666663</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="B7" s="2">
+        <v>0.70138888888888884</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -508,7 +519,7 @@
       </c>
       <c r="D32" s="2">
         <f xml:space="preserve"> SUM(D2:D31)</f>
-        <v>0.35416666666666663</v>
+        <v>0.41666666666666663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created another object, can modify the object, add outlets
too bad there isn't a doc_update() call every time
</commit_message>
<xml_diff>
--- a/hoursLog.xlsx
+++ b/hoursLog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>date</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>reacquainting myself with min organization, setting up any connect for max</t>
+  </si>
+  <si>
+    <t>able to build a project and build objects within that project, using the IDE</t>
+  </si>
+  <si>
+    <t>creating help patches for new object, how does modifying a patch work in the ecosystem. Update comes from the .xml file in the doc folder</t>
+  </si>
+  <si>
+    <t>able to create a new inlet, now working on inlets, arguments, and attributes</t>
   </si>
 </sst>
 </file>
@@ -430,12 +439,12 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="5" max="5" width="78.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="99.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -512,6 +521,112 @@
       <c r="B7" s="2">
         <v>0.70138888888888884</v>
       </c>
+      <c r="C7" s="2">
+        <v>0.74305555555555547</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" ref="D7:D20" si="0">C7-B7</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30">
+      <c r="B8" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.79861111111111116</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>4.861111111111116E-2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" s="2">
+        <v>0.34027777777777773</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>7.6388888888888951E-2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="D20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
@@ -519,7 +634,7 @@
       </c>
       <c r="D32" s="2">
         <f xml:space="preserve"> SUM(D2:D31)</f>
-        <v>0.41666666666666663</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
end of investige min
</commit_message>
<xml_diff>
--- a/hoursLog.xlsx
+++ b/hoursLog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>date</t>
   </si>
@@ -64,6 +64,18 @@
   </si>
   <si>
     <t>able to create a new inlet, now working on inlets, arguments, and attributes</t>
+  </si>
+  <si>
+    <t>2020.05.05</t>
+  </si>
+  <si>
+    <t>recreate phasor and edge, which are MSP objects (as opposed to Max objects)</t>
+  </si>
+  <si>
+    <t>now we delve into buffers. Exploring buffer~ object and index~ object first. Lots of useful guides in source &gt;&gt; min_api &gt;&gt; doc</t>
+  </si>
+  <si>
+    <t>merge branch, get latest Resonance, create new branch and start building something that includes Res</t>
   </si>
 </sst>
 </file>
@@ -439,7 +451,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -563,21 +575,48 @@
       </c>
     </row>
     <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.67013888888888884</v>
+      </c>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>3.1249999999999889E-2</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30">
+      <c r="B11" s="2">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.77430555555555547</v>
+      </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.375E-2</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:5">
+      <c r="B12" s="2">
+        <v>0.875</v>
+      </c>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.875</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -634,7 +673,7 @@
       </c>
       <c r="D32" s="2">
         <f xml:space="preserve"> SUM(D2:D31)</f>
-        <v>0.58333333333333337</v>
+        <v>-0.16666666666666674</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
include works, compiling new C++ code does not
</commit_message>
<xml_diff>
--- a/hoursLog.xlsx
+++ b/hoursLog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>date</t>
   </si>
@@ -76,6 +76,18 @@
   </si>
   <si>
     <t>merge branch, get latest Resonance, create new branch and start building something that includes Res</t>
+  </si>
+  <si>
+    <t>2020.5.06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">including no problem. The issue is linking the c files. They are not getting compiled or linked. </t>
+  </si>
+  <si>
+    <t>keep working on compiling / linking resonance in. Ok this is a problem. Also the lack of pushing nested repo is also a problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spend some time on this submodule issue. Need to do that either way. </t>
   </si>
 </sst>
 </file>
@@ -451,7 +463,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -623,21 +635,48 @@
       </c>
     </row>
     <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="D13" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>5.5555555555555525E-2</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30">
+      <c r="B14" s="2">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.18055555555555555</v>
+      </c>
       <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666657E-2</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:5">
+      <c r="C15" s="2">
+        <v>0.1875</v>
+      </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1875</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -676,7 +715,7 @@
       </c>
       <c r="D32" s="2">
         <f xml:space="preserve"> SUM(D2:D31)</f>
-        <v>0.77083333333333326</v>
+        <v>1.0555555555555554</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
now able to build resonance object files from inside min!
</commit_message>
<xml_diff>
--- a/hoursLog.xlsx
+++ b/hoursLog.xlsx
@@ -87,7 +87,7 @@
     <t>keep working on compiling / linking resonance in. Ok this is a problem. Also the lack of pushing nested repo is also a problem</t>
   </si>
   <si>
-    <t xml:space="preserve">spend some time on this submodule issue. Need to do that either way. </t>
+    <t>spend some time on this submodule issue. Need to do that either way. A quick look back at CICM Hoa, and enter flext</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -654,35 +654,41 @@
     </row>
     <row r="14" spans="1:5" ht="30">
       <c r="B14" s="2">
-        <v>0.1388888888888889</v>
+        <v>0.63888888888888895</v>
       </c>
       <c r="C14" s="2">
-        <v>0.18055555555555555</v>
+        <v>0.68055555555555547</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>4.1666666666666657E-2</v>
+        <v>4.1666666666666519E-2</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:5">
+      <c r="B15" s="2">
+        <v>0.69097222222222221</v>
+      </c>
       <c r="C15" s="2">
-        <v>0.1875</v>
+        <v>0.75347222222222221</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>0.1875</v>
+        <v>6.25E-2</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:5">
+      <c r="B16" s="2">
+        <v>0.76736111111111116</v>
+      </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.76736111111111116</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -715,7 +721,7 @@
       </c>
       <c r="D32" s="2">
         <f xml:space="preserve"> SUM(D2:D31)</f>
-        <v>1.0555555555555554</v>
+        <v>0.1631944444444442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
solid organization for adding source files to objects
</commit_message>
<xml_diff>
--- a/hoursLog.xlsx
+++ b/hoursLog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>date</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>spend some time on this submodule issue. Need to do that either way. A quick look back at CICM Hoa, and enter flext</t>
+  </si>
+  <si>
+    <t>attempt more flext, sudden idea for min and backpivot</t>
+  </si>
+  <si>
+    <t>Woohoo! Now able to build resonance object files from inside min devkit! Now work on buffer conversion</t>
   </si>
 </sst>
 </file>
@@ -123,12 +129,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,7 +472,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -686,42 +695,63 @@
       <c r="B16" s="2">
         <v>0.76736111111111116</v>
       </c>
+      <c r="C16" s="2">
+        <v>0.80208333333333337</v>
+      </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>-0.76736111111111116</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>3.472222222222221E-2</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="B17" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.88888888888888884</v>
+      </c>
       <c r="D17" s="2">
         <f t="shared" si="0"/>
+        <v>5.5555555555555469E-2</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="D18" s="2">
+    <row r="19" spans="1:5">
+      <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="D19" s="2">
+    <row r="20" spans="1:5">
+      <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="D20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+    <row r="25" spans="1:5">
+      <c r="E25" s="3">
+        <f xml:space="preserve"> SUM(D13:D16)</f>
+        <v>0.19444444444444425</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>10</v>
       </c>
       <c r="D32" s="2">
         <f xml:space="preserve"> SUM(D2:D31)</f>
-        <v>0.1631944444444442</v>
+        <v>1.020833333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed 2 channel crashes
</commit_message>
<xml_diff>
--- a/hoursLog.xlsx
+++ b/hoursLog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>date</t>
   </si>
@@ -102,7 +102,10 @@
     <t>Working on audio buffer conversion</t>
   </si>
   <si>
-    <t>more audio buffers</t>
+    <t>more audio buffers. Thru object works with 1 channel but crashes with 2</t>
+  </si>
+  <si>
+    <t>2 channel crash was because I declared buffers as mono. Drum loop is hella crackly, don't use this for testing</t>
   </si>
 </sst>
 </file>
@@ -481,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -751,20 +754,32 @@
     </row>
     <row r="19" spans="1:5">
       <c r="B19" s="2">
-        <v>0.67013888888888884</v>
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.73958333333333337</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="0"/>
-        <v>-0.67013888888888884</v>
+        <v>6.597222222222221E-2</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:5">
+      <c r="B20" s="2">
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.8125</v>
+      </c>
       <c r="D20" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.472222222222221E-2</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -776,7 +791,7 @@
       </c>
       <c r="D32" s="3">
         <f xml:space="preserve"> SUM(D2:D30)</f>
-        <v>0.4722222222222221</v>
+        <v>1.2430555555555554</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ported buffer conversion to a separate .h file
</commit_message>
<xml_diff>
--- a/hoursLog.xlsx
+++ b/hoursLog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>date</t>
   </si>
@@ -106,6 +106,21 @@
   </si>
   <si>
     <t>2 channel crash was because I declared buffers as mono. Drum loop is hella crackly, don't use this for testing</t>
+  </si>
+  <si>
+    <t>2020.05.08</t>
+  </si>
+  <si>
+    <t>look at CICM UI to prep for Konrad call, think about UI</t>
+  </si>
+  <si>
+    <t>call with Konrad</t>
+  </si>
+  <si>
+    <t>continue working on porting conversion functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linker error with conversions. Issue was that all the min stuff doesn't use implementation files, so the Only Once rule being violated in the resulting object files. </t>
   </si>
 </sst>
 </file>
@@ -484,7 +499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -571,7 +586,7 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" ref="D7:D20" si="0">C7-B7</f>
+        <f t="shared" ref="D7:D26" si="0">C7-B7</f>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -782,8 +797,81 @@
         <v>28</v>
       </c>
     </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="B22" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="0"/>
+        <v>5.2083333333333259E-2</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" s="2">
+        <v>0.71875</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30">
+      <c r="B24" s="2">
+        <v>0.84375</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" si="0"/>
+        <v>7.291666666666663E-2</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="25" spans="1:5">
+      <c r="D25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E25"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="D26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
@@ -791,7 +879,7 @@
       </c>
       <c r="D32" s="3">
         <f xml:space="preserve"> SUM(D2:D30)</f>
-        <v>1.2430555555555554</v>
+        <v>1.5347222222222219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
after git add helloWorldPackage
</commit_message>
<xml_diff>
--- a/hoursLog.xlsx
+++ b/hoursLog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>date</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t xml:space="preserve">linker error with conversions. Issue was that all the min stuff doesn't use implementation files, so the Only Once rule being violated in the resulting object files. </t>
+  </si>
+  <si>
+    <t>2020.05.11</t>
+  </si>
+  <si>
+    <t>Priority is to sort out git submodules!</t>
   </si>
 </sst>
 </file>
@@ -499,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -861,11 +867,19 @@
       </c>
     </row>
     <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.49305555555555558</v>
+      </c>
       <c r="D25" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E25"/>
+        <v>-0.49305555555555558</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="26" spans="1:5">
       <c r="D26" s="2">
@@ -879,7 +893,7 @@
       </c>
       <c r="D32" s="3">
         <f xml:space="preserve"> SUM(D2:D30)</f>
-        <v>1.5347222222222219</v>
+        <v>1.0416666666666663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed incorrect submodule add for helloWorldPackage
</commit_message>
<xml_diff>
--- a/hoursLog.xlsx
+++ b/hoursLog.xlsx
@@ -506,7 +506,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -873,9 +873,12 @@
       <c r="B25" s="2">
         <v>0.49305555555555558</v>
       </c>
+      <c r="C25" s="2">
+        <v>0.56944444444444442</v>
+      </c>
       <c r="D25" s="2">
         <f t="shared" si="0"/>
-        <v>-0.49305555555555558</v>
+        <v>7.638888888888884E-2</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>35</v>
@@ -893,7 +896,7 @@
       </c>
       <c r="D32" s="3">
         <f xml:space="preserve"> SUM(D2:D30)</f>
-        <v>1.0416666666666663</v>
+        <v>1.6111111111111107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hours log before merge
</commit_message>
<xml_diff>
--- a/hoursLog.xlsx
+++ b/hoursLog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>date</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>Priority is to sort out git submodules!</t>
+  </si>
+  <si>
+    <t>submodules are now completely sorted out</t>
   </si>
 </sst>
 </file>
@@ -506,7 +509,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -885,9 +888,18 @@
       </c>
     </row>
     <row r="26" spans="1:5">
+      <c r="B26" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.70138888888888884</v>
+      </c>
       <c r="D26" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.722222222222221E-2</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -896,7 +908,7 @@
       </c>
       <c r="D32" s="3">
         <f xml:space="preserve"> SUM(D2:D30)</f>
-        <v>1.6111111111111107</v>
+        <v>1.708333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
maybe there are git files that need to be committed
</commit_message>
<xml_diff>
--- a/hoursLog.xlsx
+++ b/hoursLog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>date</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>submodules are now completely sorted out</t>
+  </si>
+  <si>
+    <t>start working on first order encoder!</t>
   </si>
 </sst>
 </file>
@@ -139,10 +142,26 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -165,8 +184,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -176,7 +197,9 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -506,9 +529,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -595,7 +618,7 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" ref="D7:D26" si="0">C7-B7</f>
+        <f t="shared" ref="D7:D46" si="0">C7-B7</f>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -892,27 +915,36 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="C26" s="2">
-        <v>0.70138888888888884</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" si="0"/>
-        <v>9.722222222222221E-2</v>
+        <v>0.10416666666666674</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
-      <c r="A32" t="s">
+    <row r="27" spans="1:5">
+      <c r="B27" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D49" s="3">
         <f xml:space="preserve"> SUM(D2:D30)</f>
-        <v>1.708333333333333</v>
+        <v>1.7152777777777775</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>